<commit_message>
Update PDS template files
(cherry picked from commit cb48d6197a1cfd44502dc2f6d7cec0616b73ad5f)
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/Secondary_Circuit_MatchTable_Default.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/Secondary_Circuit_MatchTable_Default.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F01E08-916E-45AC-913B-F67BF59FDDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -316,7 +317,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -860,6 +861,9 @@
       <c r="E6" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -875,9 +879,6 @@
         <v>63</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="1" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>